<commit_message>
not finishhh wanna cry
</commit_message>
<xml_diff>
--- a/lab06/lab06-02.xlsx
+++ b/lab06/lab06-02.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\noey\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\noey\Desktop\github repo\ไม่ใช่ project\year2\Physical-Computing\lab06\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FEFCBE30-8416-4864-8675-DEDAC943AF43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACFB8740-8703-4CAE-9734-11D6735057C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-83" yWindow="0" windowWidth="10965" windowHeight="12863" xr2:uid="{ACC8FC54-27C0-462F-84C4-A42FC0032B2A}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{ACC8FC54-27C0-462F-84C4-A42FC0032B2A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="43">
   <si>
     <t>หลัก j = 0</t>
   </si>
@@ -138,13 +138,168 @@
   </si>
   <si>
     <t>2[2][2]</t>
+  </si>
+  <si>
+    <t>a[0][0]=1i0*2j0</t>
+  </si>
+  <si>
+    <t>a[1][0]=1[1][0]*2[0][0] + 1[1][1]*2[1][0]</t>
+  </si>
+  <si>
+    <t>a[0][0]=1[0][0]*2[0][0] + 1[0][1]*2[1][0]</t>
+  </si>
+  <si>
+    <r>
+      <t>a[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF92D050"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <charset val="222"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>][</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <charset val="222"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>]=1[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF92D050"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <charset val="222"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>][0]*2[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF92D050"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <charset val="222"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>][1] + 1[0][</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <charset val="222"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>]*2[1][</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <charset val="222"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>]</t>
+    </r>
+  </si>
+  <si>
+    <t>a[0][0]</t>
+  </si>
+  <si>
+    <t>a[0][1]</t>
+  </si>
+  <si>
+    <t>a[0][2]</t>
+  </si>
+  <si>
+    <t>a[1][0]</t>
+  </si>
+  <si>
+    <t>a[2][0]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -153,8 +308,22 @@
       <charset val="222"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF92D050"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B0F0"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -173,6 +342,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -186,11 +361,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -525,18 +704,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1233E02-5B68-4E74-8F02-4211F88DC7D1}">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:M31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="16384" width="9" style="1"/>
+    <col min="1" max="11" width="9" style="1"/>
+    <col min="12" max="12" width="37.625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="42.375" style="1" customWidth="1"/>
+    <col min="14" max="14" width="14.5625" style="1" customWidth="1"/>
+    <col min="15" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -547,7 +730,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -561,7 +744,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -575,17 +758,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B8" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B10" s="1" t="s">
         <v>13</v>
       </c>
@@ -604,8 +787,11 @@
       <c r="I10" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="L10" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
@@ -631,7 +817,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
@@ -657,7 +843,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
@@ -682,8 +868,194 @@
       <c r="I13" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="L13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="L14" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I21" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J21" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="K21" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I22" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A23" s="7">
+        <v>1</v>
+      </c>
+      <c r="B23" s="7">
+        <v>2</v>
+      </c>
+      <c r="C23" s="7">
+        <v>3</v>
+      </c>
+      <c r="E23" s="7">
+        <v>1</v>
+      </c>
+      <c r="F23" s="7">
+        <v>2</v>
+      </c>
+      <c r="G23" s="7">
+        <v>3</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A24" s="7">
+        <v>4</v>
+      </c>
+      <c r="B24" s="7">
+        <v>5</v>
+      </c>
+      <c r="C24" s="7">
+        <v>6</v>
+      </c>
+      <c r="E24" s="7">
+        <v>4</v>
+      </c>
+      <c r="F24" s="7">
+        <v>5</v>
+      </c>
+      <c r="G24" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A25" s="7">
+        <v>7</v>
+      </c>
+      <c r="B25" s="7">
+        <v>8</v>
+      </c>
+      <c r="C25" s="7">
+        <v>9</v>
+      </c>
+      <c r="E25" s="7">
+        <v>7</v>
+      </c>
+      <c r="F25" s="7">
+        <v>8</v>
+      </c>
+      <c r="G25" s="7">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A27" s="6">
+        <f>A23*E23</f>
+        <v>1</v>
+      </c>
+      <c r="B27" s="6">
+        <f>B23*E24</f>
+        <v>8</v>
+      </c>
+      <c r="C27" s="6">
+        <f>C23*E25</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A28" s="6"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A29" s="6">
+        <f>SUM(A27:C27)</f>
+        <v>30</v>
+      </c>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A30" s="6"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A31" s="6"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>